<commit_message>
- Sửa code lệnh HTK cho giống file notes K22. - Thêm dữ liệu test (270 files train + 30 files test + NewSentences.txt) - Cập nhật báo cáo.
Nhận xét: Sau khi sửa code lệnh HTK thì em test lại kết quả không khác trước khi sửa.
</commit_message>
<xml_diff>
--- a/Lab3.22/Statistic.xlsx
+++ b/Lab3.22/Statistic.xlsx
@@ -412,7 +412,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.2843</c:v>
+                  <c:v>0.27229999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.3241</c:v>
@@ -530,7 +530,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.28100000000000003</c:v>
+                  <c:v>0.28270000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.29170000000000001</c:v>
@@ -552,11 +552,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="300487776"/>
-        <c:axId val="300487384"/>
+        <c:axId val="219606560"/>
+        <c:axId val="219610480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="300487776"/>
+        <c:axId val="219606560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +599,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300487384"/>
+        <c:crossAx val="219610480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -607,7 +607,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="300487384"/>
+        <c:axId val="219610480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300487776"/>
+        <c:crossAx val="219606560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -922,7 +922,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>41.546399999999998</c:v>
+                  <c:v>45.131</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>38.001399999999997</c:v>
@@ -1040,7 +1040,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>42.595100000000002</c:v>
+                  <c:v>41.958799999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42.223300000000002</c:v>
@@ -1062,11 +1062,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="302965232"/>
-        <c:axId val="302967584"/>
+        <c:axId val="219607736"/>
+        <c:axId val="219609304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="302965232"/>
+        <c:axId val="219607736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1109,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302967584"/>
+        <c:crossAx val="219609304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1117,7 +1117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302967584"/>
+        <c:axId val="219609304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302965232"/>
+        <c:crossAx val="219607736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2690,11 +2690,12 @@
   <dimension ref="B1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
@@ -2722,19 +2723,19 @@
         <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>0.2843</v>
+        <v>0.27229999999999999</v>
       </c>
       <c r="D2" s="3">
-        <v>0.28100000000000003</v>
+        <v>0.28270000000000001</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="8">
-        <v>41.546399999999998</v>
+        <v>45.131</v>
       </c>
       <c r="M2" s="8">
-        <v>42.595100000000002</v>
+        <v>41.958799999999997</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Thống kê lại 3 mẫu với NewSentences.txt (280 câu).
</commit_message>
<xml_diff>
--- a/Lab3.22/Statistic.xlsx
+++ b/Lab3.22/Statistic.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TN1" sheetId="1" r:id="rId1"/>
+    <sheet name="TN2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>sn0001</t>
   </si>
@@ -180,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -208,6 +209,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -311,7 +315,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'TN1'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -390,7 +394,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>'TN1'!$B$2:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -407,7 +411,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:f>'TN1'!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -415,10 +419,10 @@
                   <c:v>0.27229999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3241</c:v>
+                  <c:v>0.31269999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12239999999999999</c:v>
+                  <c:v>7.3700000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -429,7 +433,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'TN1'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -508,7 +512,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>'TN1'!$B$2:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -525,7 +529,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:f>'TN1'!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -533,10 +537,10 @@
                   <c:v>0.28270000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29170000000000001</c:v>
+                  <c:v>0.30499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.105</c:v>
+                  <c:v>7.3700000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -552,11 +556,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="219606560"/>
-        <c:axId val="219610480"/>
+        <c:axId val="265071440"/>
+        <c:axId val="265072336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219606560"/>
+        <c:axId val="265071440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219610480"/>
+        <c:crossAx val="265072336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -607,7 +611,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219610480"/>
+        <c:axId val="265072336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -627,7 +631,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -658,9 +662,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219606560"/>
+        <c:crossAx val="265071440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -821,7 +826,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1</c:f>
+              <c:f>'TN1'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -900,7 +905,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$K$2:$K$4</c:f>
+              <c:f>'TN1'!$K$2:$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -917,7 +922,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$4</c:f>
+              <c:f>'TN1'!$L$2:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -925,10 +930,10 @@
                   <c:v>45.131</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.001399999999997</c:v>
+                  <c:v>36.527500000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49.415399999999998</c:v>
+                  <c:v>46.311599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -939,7 +944,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$1</c:f>
+              <c:f>'TN1'!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1018,7 +1023,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$K$2:$K$4</c:f>
+              <c:f>'TN1'!$K$2:$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1035,7 +1040,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$4</c:f>
+              <c:f>'TN1'!$M$2:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1043,10 +1048,10 @@
                   <c:v>41.958799999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.223300000000002</c:v>
+                  <c:v>38.257199999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.124200000000002</c:v>
+                  <c:v>61.240299999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1062,11 +1067,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="219607736"/>
-        <c:axId val="219609304"/>
+        <c:axId val="265170320"/>
+        <c:axId val="265179144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219607736"/>
+        <c:axId val="265170320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1114,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219609304"/>
+        <c:crossAx val="265179144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1117,7 +1122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219609304"/>
+        <c:axId val="265179144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1173,1037 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219607736"/>
+        <c:crossAx val="265170320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Kết quả xét trên từ </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TN2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bigram</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TN2'!$B$2:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>sn0001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sn0040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sn0041</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TN2'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.26179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2900000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TN2'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>trigram</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TN2'!$B$2:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>sn0001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sn0040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sn0041</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TN2'!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.25650000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2432</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.7599999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="409805416"/>
+        <c:axId val="409804632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="409805416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409804632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="409804632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409805416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Perplexity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TN2'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bigram</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TN2'!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>sn0001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sn0040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sn0041</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TN2'!$L$2:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>370.3655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>381.54820000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>344.77019999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'TN2'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>trigram</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'TN2'!$K$2:$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>sn0001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sn0040</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sn0041</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'TN2'!$M$2:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>367.41199999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>348.54989999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>401.24029999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="411779496"/>
+        <c:axId val="411781848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="411779496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411781848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="411781848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411779496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1329,6 +2364,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1833,6 +2948,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2340,15 +4461,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2370,19 +4491,84 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2689,9 +4875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2701,11 +4885,14 @@
     <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
+    <row r="1" spans="2:13" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -2743,19 +4930,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>0.3241</v>
+        <v>0.31269999999999998</v>
       </c>
       <c r="D3" s="4">
-        <v>0.29170000000000001</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="9">
-        <v>38.001399999999997</v>
+        <v>36.527500000000003</v>
       </c>
       <c r="M3" s="9">
-        <v>42.223300000000002</v>
+        <v>38.257199999999997</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2763,19 +4950,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="4">
-        <v>0.12239999999999999</v>
+        <v>7.3700000000000002E-2</v>
       </c>
       <c r="D4" s="4">
-        <v>0.105</v>
+        <v>7.3700000000000002E-2</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="8">
-        <v>49.415399999999998</v>
+        <v>46.311599999999999</v>
       </c>
       <c r="M4" s="8">
-        <v>61.124200000000002</v>
+        <v>61.240299999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2783,4 +4970,104 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.26179999999999998</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.25650000000000001</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <v>370.3655</v>
+      </c>
+      <c r="M2" s="8">
+        <v>367.41199999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.251</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.2432</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10">
+        <v>381.54820000000001</v>
+      </c>
+      <c r="M3" s="9">
+        <v>348.54989999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="8">
+        <v>344.77019999999999</v>
+      </c>
+      <c r="M4" s="8">
+        <v>401.24029999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>